<commit_message>
Added 2018 NFL Week 18 re-run results
</commit_message>
<xml_diff>
--- a/NFL2018/Weekly Forecasts/Week11.xlsx
+++ b/NFL2018/Weekly Forecasts/Week11.xlsx
@@ -212,7 +212,7 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Mexico City</t>
+    <t>Los Angeles</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.9979616118182912</v>
+        <v>0.9980067916143047</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -1014,7 +1014,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>66.60169817581688</v>
+        <v>66.60471337309711</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -1023,10 +1023,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.526572894685421</v>
+        <v>0.526276894744621</v>
       </c>
       <c r="C6" s="6">
-        <v>0.4734271053145789</v>
+        <v>0.473723105255379</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -1034,10 +1034,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>24.48609190278162</v>
+        <v>24.48160210367958</v>
       </c>
       <c r="C7" s="7">
-        <v>23.3734815253037</v>
+        <v>23.38127172374566</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -1416,31 +1416,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.8348325363745586</v>
+        <v>0.8346445004832498</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" s="5">
-        <v>0.9895953174070782</v>
+        <v>0.9895123072389107</v>
       </c>
       <c r="F4" s="5"/>
       <c r="H4" s="5">
-        <v>0.9996982035189407</v>
+        <v>0.9996937723115322</v>
       </c>
       <c r="I4" s="5"/>
       <c r="K4" s="5">
-        <v>0.8164926934106173</v>
+        <v>0.8168209664417571</v>
       </c>
       <c r="L4" s="5"/>
       <c r="N4" s="5">
-        <v>0.9774151477218441</v>
+        <v>0.9772843493862604</v>
       </c>
       <c r="O4" s="5"/>
       <c r="Q4" s="5">
-        <v>0.9959604127313363</v>
+        <v>0.9960064449161861</v>
       </c>
       <c r="R4" s="5"/>
       <c r="T4" s="5">
-        <v>0.9687711618679633</v>
+        <v>0.9690623610513455</v>
       </c>
       <c r="U4" s="5"/>
     </row>
@@ -1449,31 +1449,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>49.22980674229424</v>
+        <v>49.21871832613122</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="4">
-        <v>49.09373914153412</v>
+        <v>49.08962101418405</v>
       </c>
       <c r="F5" s="4"/>
       <c r="H5" s="4">
-        <v>21.84886258677334</v>
+        <v>21.84876574070378</v>
       </c>
       <c r="I5" s="4"/>
       <c r="K5" s="4">
-        <v>51.02712093712545</v>
+        <v>51.04763652507321</v>
       </c>
       <c r="L5" s="4"/>
       <c r="N5" s="4">
-        <v>51.76864840964206</v>
+        <v>51.76172069518707</v>
       </c>
       <c r="O5" s="4"/>
       <c r="Q5" s="4">
-        <v>52.4566860561897</v>
+        <v>52.459110545997</v>
       </c>
       <c r="R5" s="4"/>
       <c r="T5" s="4">
-        <v>39.21848088036874</v>
+        <v>39.23026941212461</v>
       </c>
       <c r="U5" s="4"/>
     </row>
@@ -1482,46 +1482,46 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.7345684530863094</v>
+        <v>0.7346964530607094</v>
       </c>
       <c r="C6" s="6">
-        <v>0.2654315469136906</v>
+        <v>0.2653035469392906</v>
       </c>
       <c r="E6" s="6">
-        <v>0.4400224119955176</v>
+        <v>0.4397842120431576</v>
       </c>
       <c r="F6" s="6">
-        <v>0.5599775880044824</v>
+        <v>0.5602157879568425</v>
       </c>
       <c r="H6" s="6">
-        <v>0.5102267979546404</v>
+        <v>0.5103015979396804</v>
       </c>
       <c r="I6" s="6">
-        <v>0.4897732020453596</v>
+        <v>0.4896984020603196</v>
       </c>
       <c r="K6" s="6">
-        <v>0.2533166493366701</v>
+        <v>0.2535272492945501</v>
       </c>
       <c r="L6" s="6">
-        <v>0.7466833506633299</v>
+        <v>0.7464727507054498</v>
       </c>
       <c r="N6" s="6">
-        <v>0.4117595176480965</v>
+        <v>0.4115057176988565</v>
       </c>
       <c r="O6" s="6">
-        <v>0.5882404823519035</v>
+        <v>0.5884942823011435</v>
       </c>
       <c r="Q6" s="6">
-        <v>0.4626007074798585</v>
+        <v>0.4628142074371585</v>
       </c>
       <c r="R6" s="6">
-        <v>0.5373992925201415</v>
+        <v>0.5371857925628415</v>
       </c>
       <c r="T6" s="6">
-        <v>0.3963430207313959</v>
+        <v>0.3968239206352159</v>
       </c>
       <c r="U6" s="6">
-        <v>0.6036569792686042</v>
+        <v>0.6031760793647841</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -1529,46 +1529,46 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>29.38686432262714</v>
+        <v>29.38457972308406</v>
       </c>
       <c r="C7" s="7">
-        <v>18.59014388197122</v>
+        <v>18.5893104821379</v>
       </c>
       <c r="E7" s="7">
-        <v>22.5281814943637</v>
+        <v>22.51861269627746</v>
       </c>
       <c r="F7" s="7">
-        <v>25.13787537242493</v>
+        <v>25.1387709722458</v>
       </c>
       <c r="H7" s="7">
-        <v>27.61262607747479</v>
+        <v>27.61247407750518</v>
       </c>
       <c r="I7" s="7">
-        <v>27.06750318649936</v>
+        <v>27.0634989873002</v>
       </c>
       <c r="K7" s="7">
-        <v>16.9800620039876</v>
+        <v>16.96889520622096</v>
       </c>
       <c r="L7" s="7">
-        <v>28.01843059631388</v>
+        <v>28.0163909967218</v>
       </c>
       <c r="N7" s="7">
-        <v>16.49105470178906</v>
+        <v>16.49035590192882</v>
       </c>
       <c r="O7" s="7">
-        <v>19.75556624888675</v>
+        <v>19.76612684677463</v>
       </c>
       <c r="Q7" s="7">
-        <v>22.14293517141297</v>
+        <v>22.1520319695936</v>
       </c>
       <c r="R7" s="7">
-        <v>23.66884046623191</v>
+        <v>23.67562226487555</v>
       </c>
       <c r="T7" s="7">
-        <v>24.51527489694502</v>
+        <v>24.52332069533586</v>
       </c>
       <c r="U7" s="7">
-        <v>29.50787309842538</v>
+        <v>29.49839610032078</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -2586,15 +2586,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.9630597801384102</v>
+        <v>0.9630498569288877</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" s="5">
-        <v>0.9826745513195485</v>
+        <v>0.9828408279543228</v>
       </c>
       <c r="F4" s="5"/>
       <c r="H4" s="5">
-        <v>0.8854499014078456</v>
+        <v>0.8851887462414938</v>
       </c>
       <c r="I4" s="5"/>
     </row>
@@ -2603,15 +2603,15 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>59.52630475810742</v>
+        <v>59.52569140885704</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="4">
-        <v>4.501612084850677</v>
+        <v>4.502373794724535</v>
       </c>
       <c r="F5" s="4"/>
       <c r="H5" s="4">
-        <v>66.92871360541307</v>
+        <v>66.90897360735384</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -2620,22 +2620,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.6126625774674845</v>
+        <v>0.6126775774644845</v>
       </c>
       <c r="C6" s="6">
-        <v>0.3873374225325155</v>
+        <v>0.3873224225355155</v>
       </c>
       <c r="E6" s="6">
-        <v>0.5773334845333031</v>
+        <v>0.576962984607403</v>
       </c>
       <c r="F6" s="6">
-        <v>0.4226665154666969</v>
+        <v>0.4230370153925969</v>
       </c>
       <c r="H6" s="6">
-        <v>0.6965645606870878</v>
+        <v>0.6967822606435479</v>
       </c>
       <c r="I6" s="6">
-        <v>0.3034354393129121</v>
+        <v>0.3032177393564521</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -2643,22 +2643,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>25.40633371873326</v>
+        <v>25.40387511922498</v>
       </c>
       <c r="C7" s="7">
-        <v>20.55911008817798</v>
+        <v>20.55211468957706</v>
       </c>
       <c r="E7" s="7">
-        <v>19.72113125577375</v>
+        <v>19.71429405714119</v>
       </c>
       <c r="F7" s="7">
-        <v>16.76394564721087</v>
+        <v>16.77086024582795</v>
       </c>
       <c r="H7" s="7">
-        <v>32.9255520148896</v>
+        <v>32.92678281464344</v>
       </c>
       <c r="I7" s="7">
-        <v>23.28955934208813</v>
+        <v>23.28401914319617</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -3168,7 +3168,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.9240904763587503</v>
+        <v>0.9233680784625269</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -3177,7 +3177,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>65.33254175862072</v>
+        <v>65.28146873933441</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -3186,10 +3186,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.6607590678481864</v>
+        <v>0.6615082676983465</v>
       </c>
       <c r="C6" s="6">
-        <v>0.3392409321518136</v>
+        <v>0.3384917323016535</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -3197,10 +3197,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>28.32826693434661</v>
+        <v>28.33735213252957</v>
       </c>
       <c r="C7" s="7">
-        <v>20.96318440736312</v>
+        <v>20.94198881160224</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -3474,7 +3474,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.9988299757469536</v>
+        <v>0.999693909046578</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -3483,7 +3483,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>95.77470244671861</v>
+        <v>95.85754232609192</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -3492,10 +3492,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.4798657040268592</v>
+        <v>0.4897007020598596</v>
       </c>
       <c r="C6" s="6">
-        <v>0.5201342959731408</v>
+        <v>0.5102992979401404</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -3503,10 +3503,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>33.48631630273674</v>
+        <v>33.60108767978247</v>
       </c>
       <c r="C7" s="7">
-        <v>34.55481368903726</v>
+        <v>34.14911097017781</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -3528,7 +3528,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="8">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:61">
@@ -3572,7 +3572,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:61">
@@ -3583,7 +3583,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="8">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:61">
@@ -3613,7 +3613,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="8">
         <v>34</v>
@@ -3649,7 +3649,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="8">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3682,7 +3682,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="8">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3690,10 +3690,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C24" s="8">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -3704,7 +3704,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="8">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3">

</xml_diff>